<commit_message>
added groupe to final table
</commit_message>
<xml_diff>
--- a/data/FC1_POSH_ICCAT_ICES.xlsx
+++ b/data/FC1_POSH_ICCAT_ICES.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,7 +392,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -414,7 +414,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -436,12 +436,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -453,17 +453,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Centrophorus granulosus</t>
+          <t>Centrophorus squamosus</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Not applicable</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -475,17 +475,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Centrophorus granulosus</t>
+          <t>Centrophorus squamosus</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -502,12 +502,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -519,12 +519,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Centrophorus squamosus</t>
+          <t>Centroscymnus coelolepis</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -541,12 +541,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Centrophorus squamosus</t>
+          <t>Centroscymnus coelolepis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -563,12 +563,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Centrophorus squamosus</t>
+          <t>Centroscymnus coelolepis</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -585,12 +585,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Centrophorus squamosus</t>
+          <t>Cetorhinus maximus</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -607,12 +607,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Centroscymnus coelolepis</t>
+          <t>Cetorhinus maximus</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -629,17 +629,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Centroscymnus coelolepis</t>
+          <t>Cetorhinus maximus</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -651,12 +651,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Centroscymnus coelolepis</t>
+          <t>Dipturus batis</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -673,17 +673,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Centroscymnus coelolepis</t>
+          <t>Dipturus batis</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -695,17 +695,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Centroscymnus coelolepis</t>
+          <t>Dipturus batis</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -717,17 +717,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Lamna nasus</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -739,17 +739,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Lamna nasus</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -761,17 +761,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Lamna nasus</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -783,17 +783,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -805,17 +805,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -827,17 +827,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dipturus batis</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -849,17 +849,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Dipturus batis</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -871,12 +871,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Dipturus batis</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -893,12 +893,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Dipturus batis</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -915,17 +915,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dipturus batis</t>
+          <t>Rostroraja alba</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -937,17 +937,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Rostroraja alba</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -959,17 +959,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Rostroraja alba</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -981,17 +981,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Squatina squatina</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1003,17 +1003,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Squatina squatina</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1025,17 +1025,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Squatina squatina</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1047,100 +1047,100 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Amblyraja radiata</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Declining</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Amblyraja radiata</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Declining</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Cetorhinus maximus</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Cetorhinus maximus</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Chimaera monstrosa</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1150,344 +1150,344 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Chimaera monstrosa</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Dalatias licha</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Dalatias licha</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Dasyatis pastinaca</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Dasyatis pastinaca</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Rostroraja alba</t>
+          <t>Dasyatis pastinaca</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Rostroraja alba</t>
+          <t>Dasyatis pastinaca</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>II*</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Rostroraja alba</t>
+          <t>Dasyatis pastinaca</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Rostroraja alba</t>
+          <t>Dasyatis pastinaca</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Rostroraja alba</t>
+          <t>Deania calcea</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Squatina squatina</t>
+          <t>Deania calcea</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Squatina squatina</t>
+          <t>Dipturus oxyrinchus</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Squatina squatina</t>
+          <t>Dipturus oxyrinchus</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Squatina squatina</t>
+          <t>Dipturus oxyrinchus</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Long</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Squatina squatina</t>
+          <t>Dipturus oxyrinchus</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>POSH</t>
+          <t>FC1 : Short</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Amblyraja radiata</t>
+          <t>Dipturus oxyrinchus</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Declining</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1509,7 +1509,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Amblyraja radiata</t>
+          <t>Dipturus oxyrinchus</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Declining</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1531,12 +1531,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Dipturus spp</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1553,12 +1553,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Dipturus spp</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1575,7 +1575,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Chimaera monstrosa</t>
+          <t>Dipturus spp</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1597,7 +1597,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Chimaera monstrosa</t>
+          <t>Dipturus spp</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1619,7 +1619,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Dalatias licha</t>
+          <t>Etmopterus spinax</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1641,7 +1641,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Dalatias licha</t>
+          <t>Etmopterus spinax</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1663,7 +1663,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Dasyatis pastinaca</t>
+          <t>Galeorhinus galeus</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1685,7 +1685,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Dasyatis pastinaca</t>
+          <t>Galeorhinus galeus</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1707,7 +1707,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Dasyatis pastinaca</t>
+          <t>Galeorhinus galeus</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1729,7 +1729,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Dasyatis pastinaca</t>
+          <t>Galeorhinus galeus</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1751,7 +1751,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Dasyatis pastinaca</t>
+          <t>Galeorhinus galeus</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1773,7 +1773,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Dasyatis pastinaca</t>
+          <t>Galeorhinus galeus</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Deania calcea</t>
+          <t>Galeus spp</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1817,7 +1817,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Deania calcea</t>
+          <t>Galeus spp</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1839,17 +1839,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Dipturus oxyrinchus</t>
+          <t>Hexanchus griseus</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1861,17 +1861,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Dipturus oxyrinchus</t>
+          <t>Hexanchus griseus</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1883,7 +1883,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Dipturus oxyrinchus</t>
+          <t>Hydrolagus mirabilis</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1905,7 +1905,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Dipturus oxyrinchus</t>
+          <t>Hydrolagus mirabilis</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1927,17 +1927,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Dipturus oxyrinchus</t>
+          <t>Leucoraja circularis</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1949,17 +1949,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Dipturus oxyrinchus</t>
+          <t>Leucoraja circularis</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1971,17 +1971,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Dipturus spp</t>
+          <t>Leucoraja circularis</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1993,17 +1993,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Dipturus spp</t>
+          <t>Leucoraja circularis</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2015,17 +2015,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Dipturus spp</t>
+          <t>Leucoraja circularis</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Declining</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2037,17 +2037,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Dipturus spp</t>
+          <t>Leucoraja circularis</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2059,17 +2059,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Etmopterus spinax</t>
+          <t>Leucoraja fullonica</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2081,12 +2081,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Etmopterus spinax</t>
+          <t>Leucoraja fullonica</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2103,12 +2103,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Galeorhinus galeus</t>
+          <t>Leucoraja fullonica</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2125,12 +2125,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Galeorhinus galeus</t>
+          <t>Leucoraja fullonica</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2147,17 +2147,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Galeorhinus galeus</t>
+          <t>Leucoraja fullonica</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2169,17 +2169,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Galeorhinus galeus</t>
+          <t>Leucoraja fullonica</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2191,17 +2191,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Galeorhinus galeus</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2213,12 +2213,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Galeorhinus galeus</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2235,7 +2235,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Galeus spp</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2257,7 +2257,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Galeus spp</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2279,17 +2279,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Hexanchus griseus</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2301,12 +2301,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Hexanchus griseus</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2323,12 +2323,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Hydrolagus mirabilis</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2345,12 +2345,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Hydrolagus mirabilis</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2367,12 +2367,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Leucoraja circularis</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2389,12 +2389,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Leucoraja circularis</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2411,12 +2411,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Leucoraja circularis</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2433,12 +2433,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Leucoraja circularis</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2455,17 +2455,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Leucoraja circularis</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Declining</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2477,17 +2477,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Leucoraja circularis</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2499,12 +2499,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Leucoraja fullonica</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2521,17 +2521,17 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Leucoraja fullonica</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2543,12 +2543,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Leucoraja fullonica</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2565,17 +2565,17 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Leucoraja fullonica</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2587,17 +2587,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Leucoraja fullonica</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2609,17 +2609,17 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Leucoraja fullonica</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2631,17 +2631,17 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Leucoraja naevus</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2653,12 +2653,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Leucoraja naevus</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2675,17 +2675,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Leucoraja naevus</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2697,12 +2697,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Leucoraja naevus</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2719,12 +2719,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Leucoraja naevus</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2741,17 +2741,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Leucoraja naevus</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2763,17 +2763,17 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Raja brachyura</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2785,17 +2785,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Raja brachyura</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2807,12 +2807,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Raja brachyura</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2829,12 +2829,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Raja brachyura</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2851,12 +2851,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Raja brachyura</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2873,17 +2873,17 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Raja brachyura</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2895,17 +2895,17 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2917,17 +2917,17 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -2939,12 +2939,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2961,12 +2961,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2983,12 +2983,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Scyliorhinus canicula</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3005,12 +3005,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Raja clavata</t>
+          <t>Scyliorhinus canicula</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3027,17 +3027,17 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Raja microocellata</t>
+          <t>Scyliorhinus canicula</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3049,12 +3049,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Raja microocellata</t>
+          <t>Scyliorhinus canicula</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3071,17 +3071,17 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Raja microocellata</t>
+          <t>Scyliorhinus canicula</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3093,17 +3093,17 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Raja microocellata</t>
+          <t>Scyliorhinus canicula</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3115,17 +3115,17 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Raja microocellata</t>
+          <t>Scyliorhinus stellaris</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3137,12 +3137,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Raja microocellata</t>
+          <t>Scyliorhinus stellaris</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3159,12 +3159,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Scyliorhinus stellaris</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3181,12 +3181,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Scyliorhinus stellaris</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3203,17 +3203,17 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Scyliorhinus stellaris</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3225,12 +3225,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Scyliorhinus stellaris</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3247,12 +3247,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Scymnodon ringens</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3269,12 +3269,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Raja montagui</t>
+          <t>Scymnodon ringens</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3291,7 +3291,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Raja undulata</t>
+          <t>Tetronarce nobiliana</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3313,7 +3313,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Raja undulata</t>
+          <t>Tetronarce nobiliana</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3323,7 +3323,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -3335,17 +3335,17 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Raja undulata</t>
+          <t>Torpedo marmorata</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -3357,17 +3357,17 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Raja undulata</t>
+          <t>Torpedo marmorata</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -3379,139 +3379,151 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Raja undulata</t>
+          <t>Isurus oxyrinchus</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>NE Atlantic</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
-        </is>
+          <t>ICCAT + GFCM</t>
+        </is>
+      </c>
+      <c r="E138">
+        <v>2019</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Raja undulata</t>
+          <t>Lamna nasus</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>NE Atlantic</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
-        </is>
+          <t>ICCAT + GFCM</t>
+        </is>
+      </c>
+      <c r="E139">
+        <v>2009</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Scyliorhinus canicula</t>
+          <t>Prionace glauca</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>NE Atlantic</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
-        </is>
+          <t>ICCAT + GFCM</t>
+        </is>
+      </c>
+      <c r="E140">
+        <v>2015</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Scyliorhinus canicula</t>
+          <t>Galeus melastomus</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>Ligurian and Tyrrhenian Seas</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
-        </is>
+          <t>ICCAT + GFCM</t>
+        </is>
+      </c>
+      <c r="E141">
+        <v>2010</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Scyliorhinus canicula</t>
+          <t>Squatina squatina</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>NE Atlantic</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Depleted</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Scyliorhinus canicula</t>
+          <t>Rostroraja alba</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>NE Atlantic</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Depleted</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Scyliorhinus canicula</t>
+          <t>Dipturus batis</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3521,151 +3533,151 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Depleted</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Scyliorhinus canicula</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>CS (North)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Scyliorhinus stellaris</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS (South)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Scyliorhinus stellaris</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>BBIC (North)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Dec</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Scyliorhinus stellaris</t>
+          <t>Raja clavata</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC (South)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Inc</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Scyliorhinus stellaris</t>
+          <t>Raja microocellata</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>CS (South)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Dec</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Scyliorhinus stellaris</t>
+          <t>Raja brachyura</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>GNS</t>
+          <t>BBIC (South)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Inc</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Scyliorhinus stellaris</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3675,231 +3687,222 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Scymnodon ringens</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>CS (South)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Scymnodon ringens</t>
+          <t>Raja montagui</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>BBIC (North)</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Dec</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Tetronarce nobiliana</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Inc</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Tetronarce nobiliana</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Inc</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Torpedo marmorata</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>BBIC (North)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>FC1 : Long</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Torpedo marmorata</t>
+          <t>Leucoraja naevus</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>BBIC</t>
+          <t>BBIC (South)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Dec</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>FC1 : Short</t>
+          <t>ICES</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Isurus oxyrinchus</t>
+          <t>Amblyraja radiata</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>NE Atlantic</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Dec</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>ICCAT + GFCM</t>
-        </is>
-      </c>
-      <c r="E158">
-        <v>2019</v>
+          <t>ICES</t>
+        </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>NE Atlantic</t>
+          <t>CS (South)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>Very Low</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>ICCAT + GFCM</t>
-        </is>
-      </c>
-      <c r="E159">
-        <v>2009</v>
+          <t>ICES</t>
+        </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Prionace glauca</t>
+          <t>Raja undulata</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>NE Atlantic</t>
+          <t>GNS</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Inc</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>ICCAT + GFCM</t>
-        </is>
-      </c>
-      <c r="E160">
-        <v>2015</v>
+          <t>ICES</t>
+        </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Galeus melastomus</t>
+          <t>Squalus acanthias</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Ligurian and Tyrrhenian Seas</t>
+          <t>NE Atlantic</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3908,449 +3911,6 @@
         </is>
       </c>
       <c r="D161" t="inlineStr">
-        <is>
-          <t>ICCAT + GFCM</t>
-        </is>
-      </c>
-      <c r="E161">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>Squatina squatina</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>NE Atlantic</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>Depleted</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Rostroraja alba</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>NE Atlantic</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>Depleted</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Dipturus batis</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>GNS</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>Depleted</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>Raja clavata</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>CS (North)</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>Raja clavata</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>CS (South)</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>Raja clavata</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>BBIC (North)</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>Raja clavata</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>BBIC (South)</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>Inc</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>Raja microocellata</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>CS (South)</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>Raja brachyura</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>BBIC (South)</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>Inc</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>Raja montagui</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>GNS</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
-      </c>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>Raja montagui</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>CS (South)</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>Raja montagui</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>BBIC (North)</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>Leucoraja naevus</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>GNS</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>Inc</t>
-        </is>
-      </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>Leucoraja naevus</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Inc</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>Leucoraja naevus</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>BBIC (North)</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>Leucoraja naevus</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>BBIC (South)</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>Amblyraja radiata</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>GNS</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>Raja undulata</t>
-        </is>
-      </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>CS (South)</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Very Low</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>Raja undulata</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>GNS</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>Inc</t>
-        </is>
-      </c>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>ICES</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>Squalus acanthias</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>NE Atlantic</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>Poor</t>
-        </is>
-      </c>
-      <c r="D181" t="inlineStr">
         <is>
           <t>ICES</t>
         </is>

</xml_diff>